<commit_message>
target by brand normalization, price = not net
</commit_message>
<xml_diff>
--- a/CTRL_summary.xlsx
+++ b/CTRL_summary.xlsx
@@ -468,13 +468,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D2" t="n">
-        <v>0.002437674949996701</v>
+        <v>0.01620836600503682</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -488,13 +488,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.01907943559089248</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -505,16 +505,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004062650444416032</v>
+        <v>0.01578171462243604</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -525,16 +525,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01494614292203182</v>
+        <v>0.01332312203061733</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -545,16 +545,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D6" t="n">
-        <v>0.008957687774144355</v>
+        <v>0.01346477273724664</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -565,16 +565,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01006162448610458</v>
+        <v>0.01418835600368253</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -588,13 +588,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D8" t="n">
-        <v>0.002185079817898043</v>
+        <v>0.01496794011661645</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -605,13 +605,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0009064380388476579</v>
+        <v>0.01548127605487817</v>
       </c>
       <c r="E9" t="n">
         <v>6</v>
@@ -625,16 +625,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01174181676949879</v>
+        <v>0.01504320374125215</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -645,16 +645,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01159658190255166</v>
+        <v>0.01784293743082227</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -665,16 +665,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D12" t="n">
-        <v>0.04959135958271878</v>
+        <v>0.05167562611600096</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -685,16 +685,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02113003831856718</v>
+        <v>0.02555534844463045</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -705,16 +705,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0038613505708178</v>
+        <v>0.06130298902552279</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -725,16 +725,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D15" t="n">
-        <v>0.003772251073935763</v>
+        <v>0.03876143115559966</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -745,16 +745,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D16" t="n">
-        <v>0.009791259763358998</v>
+        <v>0.0304830119977643</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -765,16 +765,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D17" t="n">
-        <v>0.03430247962463411</v>
+        <v>0.0235514890650516</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -785,16 +785,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03750794028022693</v>
+        <v>0.04034556706636133</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -805,16 +805,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D19" t="n">
-        <v>0.03917858168885459</v>
+        <v>0.02103160493555583</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -825,16 +825,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D20" t="n">
-        <v>0.05133955226311464</v>
+        <v>0.01042697364633213</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -845,16 +845,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01777773627850554</v>
+        <v>0.01445360764578266</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -865,16 +865,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D22" t="n">
-        <v>0.009511973668406165</v>
+        <v>0.01334235897427572</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -885,16 +885,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01744341252280638</v>
+        <v>0.07404067007213537</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -905,16 +905,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02486133466680801</v>
+        <v>0.0266396034662232</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -925,16 +925,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01767532972216241</v>
+        <v>0.05268348743561147</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -945,16 +945,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01390162722098558</v>
+        <v>0.01856665094957526</v>
       </c>
       <c r="E26" t="n">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -965,16 +965,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.0009122215636441556</v>
+        <v>0.008665474995749744</v>
       </c>
       <c r="E27" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -985,16 +985,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.002920898640091877</v>
+        <v>-0.0002588883267010184</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1005,16 +1005,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1176470588235294</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.002543227651471764</v>
+        <v>-0.00244046954847052</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1025,16 +1025,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.09411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01278537404079611</v>
+        <v>-0.008392234013148151</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1045,16 +1045,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>0.08235294117647059</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D31" t="n">
-        <v>0.03793652911033263</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1065,16 +1065,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C32" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="D32" t="n">
-        <v>0.02295976365666609</v>
+        <v>0.05074009198151998</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1085,16 +1085,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>0.04705882352941176</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02772985668435972</v>
+        <v>0.06671307952486817</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1105,16 +1105,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0.03529411764705882</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="D34" t="n">
-        <v>0.009689796771052498</v>
+        <v>0.0406891402856535</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1125,16 +1125,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>0.02352941176470588</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="D35" t="n">
-        <v>0.01057408032451178</v>
+        <v>0.03539487786189292</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1145,16 +1145,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="D36" t="n">
-        <v>0.01048849574728662</v>
+        <v>0.03062211378614402</v>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1165,16 +1165,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="D37" t="n">
-        <v>0.007565284863853067</v>
+        <v>0.01785637177701234</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1185,16 +1185,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="D38" t="n">
-        <v>0.005086593982617696</v>
+        <v>0.08357229421406683</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1205,13 +1205,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C39" t="n">
-        <v>0.02352941176470588</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03821386490513996</v>
+        <v>0.06004966290363641</v>
       </c>
       <c r="E39" t="n">
         <v>6</v>
@@ -1225,16 +1225,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01176470588235294</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01098497217924987</v>
+        <v>0.02548405202293421</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1248,13 +1248,13 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="D41" t="n">
-        <v>0.002900104574766691</v>
+        <v>0.02545585161055538</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1265,16 +1265,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C42" t="n">
-        <v>0.09411764705882353</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00373341251634286</v>
+        <v>0.0290698900120714</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1285,16 +1285,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D43" t="n">
-        <v>0.005649953860926223</v>
+        <v>0.04711037938217573</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1305,16 +1305,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D44" t="n">
-        <v>0.04956128874633102</v>
+        <v>0.02230007097634219</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1325,16 +1325,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D45" t="n">
-        <v>0.03637554187777223</v>
+        <v>0.02264563675457226</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1345,16 +1345,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02060292276037741</v>
+        <v>0.01509011583604523</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1365,16 +1365,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D47" t="n">
-        <v>0.005543812156463842</v>
+        <v>0.0160204689394776</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1385,16 +1385,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0005435502801743634</v>
+        <v>0.02263217555223956</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1405,16 +1405,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D49" t="n">
-        <v>0.001148095693118543</v>
+        <v>0.1026626195918277</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1425,16 +1425,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.703183354053132e-05</v>
+        <v>0.08011380469575941</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -1445,16 +1445,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01226898627621761</v>
+        <v>0.02736692940330539</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1465,16 +1465,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C52" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D52" t="n">
-        <v>0.008597070074865387</v>
+        <v>0.02711764494530966</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1488,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.0004561768540815202</v>
+        <v>0.0231150025931239</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -1508,13 +1508,13 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.0007555393145033808</v>
+        <v>0.008620186414239891</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -1528,13 +1528,13 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.002743167409396722</v>
+        <v>0.01082318855549162</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -1545,16 +1545,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D56" t="n">
-        <v>0.00109795582801841</v>
+        <v>-0.005322928362963982</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -1565,16 +1565,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0003613293249582918</v>
+        <v>9.807064068323003e-05</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -1585,16 +1585,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0026463571414862</v>
+        <v>0.002748929480296277</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -1605,16 +1605,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0003877977722890892</v>
+        <v>0.005349957648444544</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -1625,16 +1625,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0006747303016358669</v>
+        <v>0.002095470253078279</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
@@ -1645,16 +1645,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0006325394004079882</v>
+        <v>0.007799527912398119</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -1665,16 +1665,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D62" t="n">
-        <v>0.006434862750064889</v>
+        <v>0.00912520359381159</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
@@ -1685,16 +1685,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D63" t="n">
-        <v>0.00395292800188196</v>
+        <v>0.03898778829828757</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -1705,16 +1705,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D64" t="n">
-        <v>0.00490455907632263</v>
+        <v>0.04101507590002845</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -1725,16 +1725,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C65" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D65" t="n">
-        <v>0.009256716142577478</v>
+        <v>0.0401272033515989</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -1745,16 +1745,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D66" t="n">
-        <v>0.01254323672117837</v>
+        <v>0.01220725364471045</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C67" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.001882143979111987</v>
+        <v>0.03433937905998054</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -1785,16 +1785,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D68" t="n">
-        <v>0.003403192674011079</v>
+        <v>0.02873492659117703</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -1805,16 +1805,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D69" t="n">
-        <v>0.02756455962485001</v>
+        <v>0.02604436309537183</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
@@ -1825,16 +1825,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
+        <v>23</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.06741573033707865</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.01688352950111599</v>
+      </c>
+      <c r="E70" t="n">
         <v>12</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0.1411764705882353</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0.03083613974079381</v>
-      </c>
-      <c r="E70" t="n">
-        <v>4</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -1845,16 +1845,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D71" t="n">
-        <v>0.03454233280964683</v>
+        <v>0.03058614987803468</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
@@ -1865,16 +1865,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C72" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D72" t="n">
-        <v>0.01999446938489039</v>
+        <v>0.05035251876575056</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
@@ -1885,16 +1885,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01573732425629093</v>
+        <v>0.02854809456925302</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -1905,16 +1905,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C74" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D74" t="n">
-        <v>0.008687196379591072</v>
+        <v>0.01922080682724974</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -1925,16 +1925,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C75" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D75" t="n">
-        <v>0.008883136131359732</v>
+        <v>0.02036868223841287</v>
       </c>
       <c r="E75" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -1945,16 +1945,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D76" t="n">
-        <v>0.02514571718900015</v>
+        <v>0.0776552694842981</v>
       </c>
       <c r="E76" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -1965,16 +1965,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D77" t="n">
-        <v>0.02174887004402725</v>
+        <v>0.02414005096234412</v>
       </c>
       <c r="E77" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -1985,16 +1985,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C78" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D78" t="n">
-        <v>0.01833711692087706</v>
+        <v>0.02947504938293699</v>
       </c>
       <c r="E78" t="n">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -2005,16 +2005,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C79" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="D79" t="n">
-        <v>0.006807975841222695</v>
+        <v>0.01772201210408039</v>
       </c>
       <c r="E79" t="n">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -2025,16 +2025,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D80" t="n">
-        <v>0.00166289533042427</v>
+        <v>0.01961871975137641</v>
       </c>
       <c r="E80" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -2045,16 +2045,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00330735935981018</v>
+        <v>0.005283021182782633</v>
       </c>
       <c r="E81" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -2065,16 +2065,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D82" t="n">
-        <v>0.01746247269395677</v>
+        <v>0.08854709536729109</v>
       </c>
       <c r="E82" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -2085,16 +2085,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0288866730268521</v>
+        <v>0.05920023622291685</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -2105,16 +2105,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D84" t="n">
-        <v>0.02010476948297118</v>
+        <v>0.02019665797845099</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -2125,16 +2125,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00702453111461994</v>
+        <v>0.03648830369966845</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -2145,16 +2145,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D86" t="n">
-        <v>0.00106394913355076</v>
+        <v>0.03157927825388539</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -2165,16 +2165,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D87" t="n">
-        <v>0.00480336278860318</v>
+        <v>0.01592253483964923</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -2185,16 +2185,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D88" t="n">
-        <v>0.002329976816592303</v>
+        <v>0.04170044419646073</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F88" t="n">
         <v>18.651428571</v>
@@ -2208,13 +2208,13 @@
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D89" t="n">
-        <v>0.01089342684958521</v>
+        <v>0.0144466903088778</v>
       </c>
       <c r="E89" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F89" t="n">
         <v>43.98</v>
@@ -2225,16 +2225,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D90" t="n">
-        <v>0.004374832545153398</v>
+        <v>0.02409963119217871</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F90" t="n">
         <v>45.568571429</v>
@@ -2245,16 +2245,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0449438202247191</v>
       </c>
       <c r="D91" t="n">
-        <v>0.002425314437850298</v>
+        <v>0.03327148116476641</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F91" t="n">
         <v>83.528571429</v>
@@ -2265,16 +2265,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0.03370786516853932</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.02399357922895044</v>
+      </c>
+      <c r="E92" t="n">
         <v>8</v>
-      </c>
-      <c r="C92" t="n">
-        <v>0.1294117647058824</v>
-      </c>
-      <c r="D92" t="n">
-        <v>-0.002164504294690435</v>
-      </c>
-      <c r="E92" t="n">
-        <v>4</v>
       </c>
       <c r="F92" t="n">
         <v>87.95999999999999</v>
@@ -2285,16 +2285,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="D93" t="n">
-        <v>0.001809954060799886</v>
+        <v>0.01542668095839541</v>
       </c>
       <c r="E93" t="n">
-        <v>2.5</v>
+        <v>13</v>
       </c>
       <c r="F93" t="n">
         <v>87.95999999999999</v>
@@ -2305,16 +2305,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="D94" t="n">
-        <v>0.002257188504255344</v>
+        <v>0.01348375865814466</v>
       </c>
       <c r="E94" t="n">
-        <v>2.5</v>
+        <v>11</v>
       </c>
       <c r="F94" t="n">
         <v>87.95999999999999</v>
@@ -2325,16 +2325,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.001884938557472164</v>
+        <v>0.02026799845618994</v>
       </c>
       <c r="E95" t="n">
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="F95" t="n">
         <v>87.95999999999999</v>
@@ -2345,16 +2345,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0005584678690653593</v>
+        <v>0.0118550776560434</v>
       </c>
       <c r="E96" t="n">
-        <v>2.5</v>
+        <v>11</v>
       </c>
       <c r="F96" t="n">
         <v>87.95999999999999</v>
@@ -2368,13 +2368,13 @@
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.02247191011235955</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.0008196476953164111</v>
+        <v>0.009606751329812544</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F97" t="n">
         <v>87.95999999999999</v>
@@ -2385,16 +2385,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.03370786516853932</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0001975073633468798</v>
+        <v>0.007024210017594933</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F98" t="n">
         <v>87.95999999999999</v>
@@ -2405,16 +2405,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D99" t="n">
-        <v>0.008542583118458603</v>
+        <v>0.002961008680704502</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
         <v>76.84999999999999</v>
@@ -2425,16 +2425,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D100" t="n">
-        <v>0.003742419071212814</v>
+        <v>0.003905268781410906</v>
       </c>
       <c r="E100" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F100" t="n">
         <v>76.84999999999999</v>
@@ -2445,16 +2445,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C101" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D101" t="n">
-        <v>-0.00179648881454896</v>
+        <v>0.06831103053692548</v>
       </c>
       <c r="E101" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F101" t="n">
         <v>75.264285714</v>
@@ -2465,16 +2465,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
+        <v>15</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0.07865168539325842</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.05230509309229998</v>
+      </c>
+      <c r="E102" t="n">
         <v>7</v>
-      </c>
-      <c r="C102" t="n">
-        <v>0.1529411764705882</v>
-      </c>
-      <c r="D102" t="n">
-        <v>0.003715260180464124</v>
-      </c>
-      <c r="E102" t="n">
-        <v>2</v>
       </c>
       <c r="F102" t="n">
         <v>72.617142857</v>
@@ -2485,16 +2485,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D103" t="n">
-        <v>0.004346367490854344</v>
+        <v>0.01117323980101203</v>
       </c>
       <c r="E103" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="F103" t="n">
         <v>72.22</v>
@@ -2505,16 +2505,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D104" t="n">
-        <v>6.812733416237311e-05</v>
+        <v>-0.01111196873649376</v>
       </c>
       <c r="E104" t="n">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="F104" t="n">
         <v>72.22</v>
@@ -2528,13 +2528,13 @@
         <v>0</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D105" t="n">
-        <v>0.0002793221157102214</v>
+        <v>-0.0003900565497205171</v>
       </c>
       <c r="E105" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F105" t="n">
         <v>51.85</v>
@@ -2548,13 +2548,13 @@
         <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D106" t="n">
-        <v>0.0004777066775761256</v>
+        <v>0.003751735880393943</v>
       </c>
       <c r="E106" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F106" t="n">
         <v>51.85</v>
@@ -2565,16 +2565,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
+        <v>0</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0.06741573033707865</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.002484968200863584</v>
+      </c>
+      <c r="E107" t="n">
         <v>16</v>
-      </c>
-      <c r="C107" t="n">
-        <v>0.1411764705882353</v>
-      </c>
-      <c r="D107" t="n">
-        <v>0.03778733060492338</v>
-      </c>
-      <c r="E107" t="n">
-        <v>4</v>
       </c>
       <c r="F107" t="n">
         <v>50.264285714</v>
@@ -2585,16 +2585,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D108" t="n">
-        <v>0.01173925917662048</v>
+        <v>-2.451766017072745e-05</v>
       </c>
       <c r="E108" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F108" t="n">
         <v>46.3</v>
@@ -2605,16 +2605,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D109" t="n">
-        <v>0.002663272823064753</v>
+        <v>0.003155647981900759</v>
       </c>
       <c r="E109" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F109" t="n">
         <v>46.3</v>
@@ -2625,16 +2625,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D110" t="n">
-        <v>0.005109347817921268</v>
+        <v>0.002365223474098167</v>
       </c>
       <c r="E110" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F110" t="n">
         <v>46.3</v>
@@ -2645,16 +2645,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D111" t="n">
-        <v>0.003632254264798749</v>
+        <v>0.003294242999343921</v>
       </c>
       <c r="E111" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F111" t="n">
         <v>46.3</v>
@@ -2665,16 +2665,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D112" t="n">
-        <v>0.00128150910474453</v>
+        <v>-0.001484006929504954</v>
       </c>
       <c r="E112" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F112" t="n">
         <v>47.092857143</v>
@@ -2685,16 +2685,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D113" t="n">
-        <v>0.04166407477706914</v>
+        <v>0.00837164534354347</v>
       </c>
       <c r="E113" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F113" t="n">
         <v>48.15</v>
@@ -2705,16 +2705,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D114" t="n">
-        <v>0.04541542622075904</v>
+        <v>0.007398513472714465</v>
       </c>
       <c r="E114" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F114" t="n">
         <v>48.15</v>
@@ -2725,16 +2725,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D115" t="n">
-        <v>0.01511243422944563</v>
+        <v>0.004965966347471338</v>
       </c>
       <c r="E115" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F115" t="n">
         <v>48.015714286</v>
@@ -2745,16 +2745,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C116" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D116" t="n">
-        <v>0.0014449953564092</v>
+        <v>-0.000366043576536944</v>
       </c>
       <c r="E116" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F116" t="n">
         <v>48.61</v>
@@ -2768,13 +2768,13 @@
         <v>0</v>
       </c>
       <c r="C117" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D117" t="n">
-        <v>-0.0002356552773537571</v>
+        <v>0.004125837112216477</v>
       </c>
       <c r="E117" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F117" t="n">
         <v>48.61</v>
@@ -2785,16 +2785,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D118" t="n">
-        <v>-0.0003708560320922171</v>
+        <v>-0.002898471539957766</v>
       </c>
       <c r="E118" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F118" t="n">
         <v>47.818571429</v>
@@ -2805,16 +2805,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D119" t="n">
-        <v>0.00181967023400513</v>
+        <v>0.05703147204677034</v>
       </c>
       <c r="E119" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F119" t="n">
         <v>49.54</v>
@@ -2825,16 +2825,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D120" t="n">
-        <v>0.03167407367187682</v>
+        <v>0.02309490543897385</v>
       </c>
       <c r="E120" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F120" t="n">
         <v>47.951428571</v>
@@ -2845,16 +2845,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C121" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D121" t="n">
-        <v>0.02325131487667814</v>
+        <v>0.02887051513205706</v>
       </c>
       <c r="E121" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F121" t="n">
         <v>45.568571429</v>
@@ -2865,16 +2865,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C122" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D122" t="n">
-        <v>0.02369304310144036</v>
+        <v>0.01976643849777286</v>
       </c>
       <c r="E122" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F122" t="n">
         <v>49.54</v>
@@ -2885,16 +2885,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C123" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D123" t="n">
-        <v>0.02763875377254164</v>
+        <v>0.01215742224672788</v>
       </c>
       <c r="E123" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F123" t="n">
         <v>62.037142857</v>
@@ -2905,16 +2905,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C124" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D124" t="n">
-        <v>0.01774588829390188</v>
+        <v>-0.008353393768949098</v>
       </c>
       <c r="E124" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F124" t="n">
         <v>78.7</v>
@@ -2925,16 +2925,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C125" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D125" t="n">
-        <v>0.003445723832978797</v>
+        <v>0.01779378782282884</v>
       </c>
       <c r="E125" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F125" t="n">
         <v>78.7</v>
@@ -2945,16 +2945,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D126" t="n">
-        <v>0.005274423260598064</v>
+        <v>0.005041119631806206</v>
       </c>
       <c r="E126" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F126" t="n">
         <v>78.7</v>
@@ -2965,16 +2965,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C127" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D127" t="n">
-        <v>0.002435684459673785</v>
+        <v>0.002283211839291302</v>
       </c>
       <c r="E127" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="F127" t="n">
         <v>77.642857143</v>
@@ -2985,16 +2985,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="C128" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D128" t="n">
-        <v>0.02299958822411221</v>
+        <v>0.06553210252928482</v>
       </c>
       <c r="E128" t="n">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F128" t="n">
         <v>75</v>
@@ -3005,16 +3005,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D129" t="n">
-        <v>0.01884874974801482</v>
+        <v>0.02483776474060224</v>
       </c>
       <c r="E129" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F129" t="n">
         <v>75</v>
@@ -3025,16 +3025,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C130" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D130" t="n">
-        <v>0.02057709826094441</v>
+        <v>0.005959571070218626</v>
       </c>
       <c r="E130" t="n">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F130" t="n">
         <v>65.477142857</v>
@@ -3045,16 +3045,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C131" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="D131" t="n">
-        <v>0.01418674774741201</v>
+        <v>-0.008835108897149627</v>
       </c>
       <c r="E131" t="n">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F131" t="n">
         <v>63.89</v>
@@ -3065,16 +3065,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.101123595505618</v>
       </c>
       <c r="D132" t="n">
-        <v>0.005331025503547773</v>
+        <v>0.000241827747137712</v>
       </c>
       <c r="E132" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F132" t="n">
         <v>63.89</v>
@@ -3085,16 +3085,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C133" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0898876404494382</v>
       </c>
       <c r="D133" t="n">
-        <v>0.002640671053001069</v>
+        <v>-0.002923026313801807</v>
       </c>
       <c r="E133" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F133" t="n">
         <v>63.89</v>
@@ -3105,16 +3105,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C134" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D134" t="n">
-        <v>0.01660909501744489</v>
+        <v>0.00565699620368226</v>
       </c>
       <c r="E134" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F134" t="n">
         <v>63.89</v>
@@ -3125,16 +3125,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C135" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D135" t="n">
-        <v>0.03638920783268147</v>
+        <v>0.003706009068294575</v>
       </c>
       <c r="E135" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F135" t="n">
         <v>63.89</v>
@@ -3145,16 +3145,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D136" t="n">
-        <v>0.02468522351671784</v>
+        <v>0.009589315878933542</v>
       </c>
       <c r="E136" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F136" t="n">
         <v>63.89</v>
@@ -3165,16 +3165,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D137" t="n">
-        <v>0.0092389451671522</v>
+        <v>0.09288540589208413</v>
       </c>
       <c r="E137" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F137" t="n">
         <v>63.89</v>
@@ -3185,16 +3185,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D138" t="n">
-        <v>0.001781193992222594</v>
+        <v>0.06792467667994365</v>
       </c>
       <c r="E138" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F138" t="n">
         <v>60.19</v>
@@ -3205,16 +3205,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D139" t="n">
-        <v>0.0423276384649877</v>
+        <v>0.02165580840607882</v>
       </c>
       <c r="E139" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F139" t="n">
         <v>60.19</v>
@@ -3225,16 +3225,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D140" t="n">
-        <v>0.007778070734824855</v>
+        <v>0.00581293782952073</v>
       </c>
       <c r="E140" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F140" t="n">
         <v>64.552857143</v>
@@ -3245,16 +3245,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D141" t="n">
-        <v>0.009290745794842011</v>
+        <v>0.001739549616331494</v>
       </c>
       <c r="E141" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F141" t="n">
         <v>66.00714285700001</v>
@@ -3265,16 +3265,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D142" t="n">
-        <v>0.005218256361147928</v>
+        <v>-0.003385234266649587</v>
       </c>
       <c r="E142" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F142" t="n">
         <v>65.61</v>
@@ -3288,13 +3288,13 @@
         <v>0</v>
       </c>
       <c r="C143" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D143" t="n">
-        <v>-0.0003221390198496134</v>
+        <v>-0.002318178574782634</v>
       </c>
       <c r="E143" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F143" t="n">
         <v>65.61</v>
@@ -3305,16 +3305,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D144" t="n">
-        <v>0.01195545573602142</v>
+        <v>0.003763155531557404</v>
       </c>
       <c r="E144" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F144" t="n">
         <v>69.577142857</v>
@@ -3325,16 +3325,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C145" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D145" t="n">
-        <v>0.0076394863040195</v>
+        <v>0.04770140777616311</v>
       </c>
       <c r="E145" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F145" t="n">
         <v>68.52</v>
@@ -3348,13 +3348,13 @@
         <v>0</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D146" t="n">
-        <v>0.03120819497867222</v>
+        <v>0.01094555958575897</v>
       </c>
       <c r="E146" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F146" t="n">
         <v>74.471428571</v>
@@ -3365,16 +3365,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C147" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D147" t="n">
-        <v>0.02026337723711574</v>
+        <v>-0.0002825920293719543</v>
       </c>
       <c r="E147" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F147" t="n">
         <v>75</v>
@@ -3385,16 +3385,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C148" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D148" t="n">
-        <v>0.01679878575462652</v>
+        <v>0.00475284659945587</v>
       </c>
       <c r="E148" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F148" t="n">
         <v>75</v>
@@ -3408,13 +3408,13 @@
         <v>0</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.05617977528089887</v>
       </c>
       <c r="D149" t="n">
-        <v>0.01704917158010017</v>
+        <v>0.003740883457996265</v>
       </c>
       <c r="E149" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F149" t="n">
         <v>75</v>
@@ -3425,16 +3425,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C150" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D150" t="n">
-        <v>0.008906901393395212</v>
+        <v>0.002117071371390198</v>
       </c>
       <c r="E150" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F150" t="n">
         <v>63.89</v>
@@ -3445,16 +3445,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D151" t="n">
-        <v>0.01912165225246047</v>
+        <v>0.04788364974666999</v>
       </c>
       <c r="E151" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F151" t="n">
         <v>63.89</v>
@@ -3465,16 +3465,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C152" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D152" t="n">
-        <v>0.01604441312553097</v>
+        <v>0.008166634407153952</v>
       </c>
       <c r="E152" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F152" t="n">
         <v>57.275714286</v>
@@ -3488,13 +3488,13 @@
         <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D153" t="n">
-        <v>0.002351340470293178</v>
+        <v>0.005009978396257156</v>
       </c>
       <c r="E153" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F153" t="n">
         <v>54.63</v>
@@ -3505,13 +3505,13 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C154" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D154" t="n">
-        <v>-0.0009081685558169261</v>
+        <v>0.06873823397303497</v>
       </c>
       <c r="E154" t="n">
         <v>7</v>
@@ -3525,16 +3525,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C155" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D155" t="n">
-        <v>0.007826482013880004</v>
+        <v>0.0428339432243767</v>
       </c>
       <c r="E155" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F155" t="n">
         <v>54.63</v>
@@ -3545,16 +3545,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="C156" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.07865168539325842</v>
       </c>
       <c r="D156" t="n">
-        <v>0.004874865433115444</v>
+        <v>0.003457410237153047</v>
       </c>
       <c r="E156" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F156" t="n">
         <v>53.571428571</v>
@@ -3565,16 +3565,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C157" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D157" t="n">
-        <v>0.002061891800982244</v>
+        <v>-0.008631861697810654</v>
       </c>
       <c r="E157" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F157" t="n">
         <v>47.22</v>
@@ -3585,16 +3585,16 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.06741573033707865</v>
       </c>
       <c r="D158" t="n">
-        <v>-0.0005154729502455903</v>
+        <v>0.001130368117487659</v>
       </c>
       <c r="E158" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F158" t="n">
         <v>46.227142857</v>

</xml_diff>

<commit_message>
implemented first adaptions in terms of input dfs
</commit_message>
<xml_diff>
--- a/CTRL_summary.xlsx
+++ b/CTRL_summary.xlsx
@@ -2097,7 +2097,7 @@
         <v>9</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v>4.448</v>
       </c>
     </row>
     <row r="84">
@@ -2117,7 +2117,7 @@
         <v>7</v>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="85">
@@ -2137,7 +2137,7 @@
         <v>3</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="86">
@@ -2157,7 +2157,7 @@
         <v>4</v>
       </c>
       <c r="F86" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="87">
@@ -2177,7 +2177,7 @@
         <v>6</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="88">
@@ -2197,7 +2197,7 @@
         <v>7</v>
       </c>
       <c r="F88" t="n">
-        <v>18.651428571</v>
+        <v>18.65142857</v>
       </c>
     </row>
     <row r="89">
@@ -2237,7 +2237,7 @@
         <v>4</v>
       </c>
       <c r="F90" t="n">
-        <v>45.568571429</v>
+        <v>45.56857143</v>
       </c>
     </row>
     <row r="91">
@@ -2257,7 +2257,7 @@
         <v>3</v>
       </c>
       <c r="F91" t="n">
-        <v>83.528571429</v>
+        <v>83.52857143</v>
       </c>
     </row>
     <row r="92">
@@ -2457,7 +2457,7 @@
         <v>3</v>
       </c>
       <c r="F101" t="n">
-        <v>75.264285714</v>
+        <v>75.26428571</v>
       </c>
     </row>
     <row r="102">
@@ -2477,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="F102" t="n">
-        <v>72.617142857</v>
+        <v>72.61714286</v>
       </c>
     </row>
     <row r="103">
@@ -2577,7 +2577,7 @@
         <v>4</v>
       </c>
       <c r="F107" t="n">
-        <v>50.264285714</v>
+        <v>50.26428571</v>
       </c>
     </row>
     <row r="108">
@@ -2677,7 +2677,7 @@
         <v>4</v>
       </c>
       <c r="F112" t="n">
-        <v>47.092857143</v>
+        <v>47.09285714</v>
       </c>
     </row>
     <row r="113">
@@ -2737,7 +2737,7 @@
         <v>5</v>
       </c>
       <c r="F115" t="n">
-        <v>48.015714286</v>
+        <v>48.01571429</v>
       </c>
     </row>
     <row r="116">
@@ -2797,7 +2797,7 @@
         <v>2</v>
       </c>
       <c r="F118" t="n">
-        <v>47.818571429</v>
+        <v>47.81857143</v>
       </c>
     </row>
     <row r="119">
@@ -2837,7 +2837,7 @@
         <v>4</v>
       </c>
       <c r="F120" t="n">
-        <v>47.951428571</v>
+        <v>47.95142857</v>
       </c>
     </row>
     <row r="121">
@@ -2857,7 +2857,7 @@
         <v>2</v>
       </c>
       <c r="F121" t="n">
-        <v>45.568571429</v>
+        <v>45.56857143</v>
       </c>
     </row>
     <row r="122">
@@ -2897,7 +2897,7 @@
         <v>4</v>
       </c>
       <c r="F123" t="n">
-        <v>62.037142857</v>
+        <v>62.03714286</v>
       </c>
     </row>
     <row r="124">
@@ -2977,7 +2977,7 @@
         <v>6</v>
       </c>
       <c r="F127" t="n">
-        <v>77.642857143</v>
+        <v>77.64285714</v>
       </c>
     </row>
     <row r="128">
@@ -3037,7 +3037,7 @@
         <v>21</v>
       </c>
       <c r="F130" t="n">
-        <v>65.477142857</v>
+        <v>65.47714286</v>
       </c>
     </row>
     <row r="131">
@@ -3237,7 +3237,7 @@
         <v>2</v>
       </c>
       <c r="F140" t="n">
-        <v>64.552857143</v>
+        <v>64.55285714</v>
       </c>
     </row>
     <row r="141">
@@ -3257,7 +3257,7 @@
         <v>3</v>
       </c>
       <c r="F141" t="n">
-        <v>66.00714285700001</v>
+        <v>66.00714286</v>
       </c>
     </row>
     <row r="142">
@@ -3317,7 +3317,7 @@
         <v>4</v>
       </c>
       <c r="F144" t="n">
-        <v>69.577142857</v>
+        <v>69.57714286</v>
       </c>
     </row>
     <row r="145">
@@ -3357,7 +3357,7 @@
         <v>3</v>
       </c>
       <c r="F146" t="n">
-        <v>74.471428571</v>
+        <v>74.47142857</v>
       </c>
     </row>
     <row r="147">
@@ -3477,7 +3477,7 @@
         <v>5</v>
       </c>
       <c r="F152" t="n">
-        <v>57.275714286</v>
+        <v>57.27571429</v>
       </c>
     </row>
     <row r="153">
@@ -3557,7 +3557,7 @@
         <v>3</v>
       </c>
       <c r="F156" t="n">
-        <v>53.571428571</v>
+        <v>53.57142857</v>
       </c>
     </row>
     <row r="157">
@@ -3597,7 +3597,7 @@
         <v>2</v>
       </c>
       <c r="F158" t="n">
-        <v>46.227142857</v>
+        <v>46.22714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finsihed inserting new data
</commit_message>
<xml_diff>
--- a/CTRL_summary.xlsx
+++ b/CTRL_summary.xlsx
@@ -465,16 +465,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D2" t="n">
-        <v>0.002437674949996701</v>
+        <v>0.01118430589984052</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -485,16 +485,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.04489220743567714</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -505,16 +505,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004062650444416032</v>
+        <v>0.02030376365932415</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -525,16 +525,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01494614292203182</v>
+        <v>0.01141338170421193</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -545,16 +545,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D6" t="n">
-        <v>0.008957687774144355</v>
+        <v>-0.006942254469474616</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -565,16 +565,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01006162448610458</v>
+        <v>0.02288468778394557</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -585,16 +585,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D8" t="n">
-        <v>0.002185079817898043</v>
+        <v>0.01148581168291831</v>
       </c>
       <c r="E8" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -605,16 +605,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0009064380388476579</v>
+        <v>0.01033465832326398</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -625,16 +625,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01174181676949879</v>
+        <v>0.01041982759822606</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -645,16 +645,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01159658190255166</v>
+        <v>0.01491878149848453</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -665,16 +665,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D12" t="n">
-        <v>0.04959135958271878</v>
+        <v>0.01043451825257207</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -685,16 +685,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1411764705882353</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02113003831856718</v>
+        <v>0.007023504440674107</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -705,16 +705,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0038613505708178</v>
+        <v>0.007820833146087103</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -725,16 +725,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D15" t="n">
-        <v>0.003772251073935763</v>
+        <v>0.008690585191936122</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -745,16 +745,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D16" t="n">
-        <v>0.009791259763358998</v>
+        <v>0.01055448488542959</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -765,16 +765,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D17" t="n">
-        <v>0.03430247962463411</v>
+        <v>0.01206092087226486</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -785,16 +785,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03750794028022693</v>
+        <v>0.009691637397433317</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -805,16 +805,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D19" t="n">
-        <v>0.03917858168885459</v>
+        <v>0.01089774698983685</v>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -825,16 +825,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D20" t="n">
-        <v>0.05133955226311464</v>
+        <v>0.009684005781253682</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -845,16 +845,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01777773627850554</v>
+        <v>0.004505032532613161</v>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -865,16 +865,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D22" t="n">
-        <v>0.009511973668406165</v>
+        <v>0.009789435764383091</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -885,16 +885,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01744341252280638</v>
+        <v>0.007896089336321582</v>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -905,16 +905,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02486133466680801</v>
+        <v>0.04463257588880598</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -925,16 +925,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01767532972216241</v>
+        <v>0.007825310557779599</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -945,16 +945,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01390162722098558</v>
+        <v>0.005830171586509581</v>
       </c>
       <c r="E26" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -965,16 +965,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.0009122215636441556</v>
+        <v>0.00437113444692316</v>
       </c>
       <c r="E27" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -985,16 +985,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.002920898640091877</v>
+        <v>0.002545820485515261</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1005,16 +1005,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1176470588235294</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.002543227651471764</v>
+        <v>0.003197490231616198</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1025,16 +1025,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C30" t="n">
-        <v>0.09411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01278537404079611</v>
+        <v>0.005302044169953019</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1045,16 +1045,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>0.08235294117647059</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D31" t="n">
-        <v>0.03793652911033263</v>
+        <v>0.005704508042787212</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1065,16 +1065,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C32" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D32" t="n">
-        <v>0.02295976365666609</v>
+        <v>0.009090172517134055</v>
       </c>
       <c r="E32" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1085,16 +1085,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C33" t="n">
-        <v>0.04705882352941176</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02772985668435972</v>
+        <v>0.007606325146227353</v>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1105,16 +1105,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C34" t="n">
-        <v>0.03529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D34" t="n">
-        <v>0.009689796771052498</v>
+        <v>0.007307142415619871</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1125,16 +1125,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C35" t="n">
-        <v>0.02352941176470588</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D35" t="n">
-        <v>0.01057408032451178</v>
+        <v>0.006653400945457578</v>
       </c>
       <c r="E35" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1145,16 +1145,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C36" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D36" t="n">
-        <v>0.01048849574728662</v>
+        <v>0.007690430348873847</v>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1165,16 +1165,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D37" t="n">
-        <v>0.007565284863853067</v>
+        <v>0.006448453933323168</v>
       </c>
       <c r="E37" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1185,16 +1185,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D38" t="n">
-        <v>0.005086593982617696</v>
+        <v>0.008200075498693608</v>
       </c>
       <c r="E38" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1205,16 +1205,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C39" t="n">
-        <v>0.02352941176470588</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03821386490513996</v>
+        <v>0.01178235339397138</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1225,16 +1225,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01176470588235294</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01098497217924987</v>
+        <v>0.02844714076958525</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1245,16 +1245,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C41" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D41" t="n">
-        <v>0.002900104574766691</v>
+        <v>0.01080954111593122</v>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1265,16 +1265,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C42" t="n">
-        <v>0.09411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00373341251634286</v>
+        <v>0.007825440334571283</v>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1285,16 +1285,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D43" t="n">
-        <v>0.005649953860926223</v>
+        <v>0.01378572695054878</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1305,16 +1305,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D44" t="n">
-        <v>0.04956128874633102</v>
+        <v>0.02715259814087369</v>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1325,16 +1325,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D45" t="n">
-        <v>0.03637554187777223</v>
+        <v>0.03569393226003413</v>
       </c>
       <c r="E45" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1345,16 +1345,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02060292276037741</v>
+        <v>0.03088047603857828</v>
       </c>
       <c r="E46" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1365,16 +1365,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D47" t="n">
-        <v>0.005543812156463842</v>
+        <v>0.02579766790691434</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1385,16 +1385,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0005435502801743634</v>
+        <v>0.0105822329735973</v>
       </c>
       <c r="E48" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1405,16 +1405,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D49" t="n">
-        <v>0.001148095693118543</v>
+        <v>0.01790255139203105</v>
       </c>
       <c r="E49" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1425,16 +1425,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D50" t="n">
-        <v>-1.703183354053132e-05</v>
+        <v>0.01386153067190398</v>
       </c>
       <c r="E50" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -1445,16 +1445,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01226898627621761</v>
+        <v>0.01400517204100869</v>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1465,16 +1465,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="C52" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D52" t="n">
-        <v>0.008597070074865387</v>
+        <v>0.0143223944506718</v>
       </c>
       <c r="E52" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1485,16 +1485,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.0004561768540815202</v>
+        <v>0.01179564814916764</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -1505,16 +1505,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C54" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.0007555393145033808</v>
+        <v>0.006542962425941732</v>
       </c>
       <c r="E54" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -1525,16 +1525,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.002743167409396722</v>
+        <v>0.03464152064965953</v>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -1545,16 +1545,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D56" t="n">
-        <v>0.00109795582801841</v>
+        <v>0.02264941868386761</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -1565,19 +1565,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0003613293249582918</v>
+        <v>0.008371128671742719</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>4.448</v>
       </c>
     </row>
     <row r="58">
@@ -1585,19 +1585,19 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0026463571414862</v>
+        <v>0.006269717046145053</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="59">
@@ -1605,19 +1605,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0003877977722890892</v>
+        <v>0.00318567247486958</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="60">
@@ -1625,19 +1625,19 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C60" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0006747303016358669</v>
+        <v>0.0002767931389714694</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="61">
@@ -1645,19 +1645,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D61" t="n">
-        <v>0.0006325394004079882</v>
+        <v>-0.0002869853509251468</v>
       </c>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="62">
@@ -1665,19 +1665,19 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D62" t="n">
-        <v>0.006434862750064889</v>
+        <v>-0.0002720456314996333</v>
       </c>
       <c r="E62" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>18.651428571</v>
       </c>
     </row>
     <row r="63">
@@ -1685,19 +1685,19 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D63" t="n">
-        <v>0.00395292800188196</v>
+        <v>0.003571348907385504</v>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="64">
@@ -1705,19 +1705,19 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D64" t="n">
-        <v>0.00490455907632263</v>
+        <v>0.002331480227889832</v>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v>45.568571429</v>
       </c>
     </row>
     <row r="65">
@@ -1725,19 +1725,19 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D65" t="n">
-        <v>0.009256716142577478</v>
+        <v>-3.527607193329877e-05</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>83.528571429</v>
       </c>
     </row>
     <row r="66">
@@ -1745,19 +1745,19 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D66" t="n">
-        <v>0.01254323672117837</v>
+        <v>-0.0005569389141133346</v>
       </c>
       <c r="E66" t="n">
-        <v>4</v>
+        <v>20.5</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="67">
@@ -1765,19 +1765,19 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C67" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.001882143979111987</v>
+        <v>0.003639806497956753</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>23.5</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="68">
@@ -1785,19 +1785,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D68" t="n">
-        <v>0.003403192674011079</v>
+        <v>0.004696267324961371</v>
       </c>
       <c r="E68" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="69">
@@ -1805,19 +1805,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D69" t="n">
-        <v>0.02756455962485001</v>
+        <v>0.002267929313189486</v>
       </c>
       <c r="E69" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="70">
@@ -1825,19 +1825,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D70" t="n">
-        <v>0.03083613974079381</v>
+        <v>0.001299394348995923</v>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>22.5</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="71">
@@ -1845,19 +1845,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C71" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D71" t="n">
-        <v>0.03454233280964683</v>
+        <v>0.00212934198648457</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>25.5</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="72">
@@ -1865,19 +1865,19 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C72" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D72" t="n">
-        <v>0.01999446938489039</v>
+        <v>0.001377083796975972</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>26.5</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="73">
@@ -1885,19 +1885,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01573732425629093</v>
+        <v>0.002981657044506518</v>
       </c>
       <c r="E73" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>76.84999999999999</v>
       </c>
     </row>
     <row r="74">
@@ -1905,19 +1905,19 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C74" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D74" t="n">
-        <v>0.008687196379591072</v>
+        <v>0.001890622948251248</v>
       </c>
       <c r="E74" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>76.84999999999999</v>
       </c>
     </row>
     <row r="75">
@@ -1925,19 +1925,19 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
+        <v>5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="D75" t="n">
+        <v>-6.482993427956871e-05</v>
+      </c>
+      <c r="E75" t="n">
         <v>21</v>
       </c>
-      <c r="C75" t="n">
-        <v>0.1411764705882353</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.008883136131359732</v>
-      </c>
-      <c r="E75" t="n">
-        <v>9</v>
-      </c>
       <c r="F75" t="n">
-        <v>0</v>
+        <v>75.264285714</v>
       </c>
     </row>
     <row r="76">
@@ -1945,19 +1945,19 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D76" t="n">
-        <v>0.02514571718900015</v>
+        <v>0.03743306260835856</v>
       </c>
       <c r="E76" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>72.617142857</v>
       </c>
     </row>
     <row r="77">
@@ -1965,19 +1965,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D77" t="n">
-        <v>0.02174887004402725</v>
+        <v>0.005197993886685044</v>
       </c>
       <c r="E77" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>72.22</v>
       </c>
     </row>
     <row r="78">
@@ -1985,19 +1985,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C78" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D78" t="n">
-        <v>0.01833711692087706</v>
+        <v>0.001983272616301942</v>
       </c>
       <c r="E78" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>72.22</v>
       </c>
     </row>
     <row r="79">
@@ -2005,19 +2005,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C79" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D79" t="n">
-        <v>0.006807975841222695</v>
+        <v>0.0001411042877328555</v>
       </c>
       <c r="E79" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="80">
@@ -2025,19 +2025,19 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C80" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D80" t="n">
-        <v>0.00166289533042427</v>
+        <v>0.0002904243942506539</v>
       </c>
       <c r="E80" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="81">
@@ -2045,19 +2045,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00330735935981018</v>
+        <v>-0.0008273607067611426</v>
       </c>
       <c r="E81" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>50.264285714</v>
       </c>
     </row>
     <row r="82">
@@ -2065,19 +2065,19 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D82" t="n">
-        <v>0.01746247269395677</v>
+        <v>-0.001414245312102238</v>
       </c>
       <c r="E82" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="83">
@@ -2085,19 +2085,19 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D83" t="n">
-        <v>0.0288866730268521</v>
+        <v>-0.0007213864818561709</v>
       </c>
       <c r="E83" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F83" t="n">
-        <v>4.448</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="84">
@@ -2105,19 +2105,19 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D84" t="n">
-        <v>0.02010476948297118</v>
+        <v>0.004376896017556402</v>
       </c>
       <c r="E84" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="F84" t="n">
-        <v>5.56</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="85">
@@ -2125,19 +2125,19 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00702453111461994</v>
+        <v>0.002639431139571133</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="F85" t="n">
-        <v>5.56</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="86">
@@ -2145,19 +2145,19 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D86" t="n">
-        <v>0.00106394913355076</v>
+        <v>0.0007634974224028804</v>
       </c>
       <c r="E86" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="F86" t="n">
-        <v>5.56</v>
+        <v>47.092857143</v>
       </c>
     </row>
     <row r="87">
@@ -2165,19 +2165,19 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D87" t="n">
-        <v>0.00480336278860318</v>
+        <v>0.002503560850889579</v>
       </c>
       <c r="E87" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F87" t="n">
-        <v>5.56</v>
+        <v>48.15</v>
       </c>
     </row>
     <row r="88">
@@ -2185,19 +2185,19 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D88" t="n">
-        <v>0.002329976816592303</v>
+        <v>0.005358659026915535</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F88" t="n">
-        <v>18.65142857</v>
+        <v>48.15</v>
       </c>
     </row>
     <row r="89">
@@ -2205,19 +2205,19 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D89" t="n">
-        <v>0.01089342684958521</v>
+        <v>0.002284018263936385</v>
       </c>
       <c r="E89" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F89" t="n">
-        <v>43.98</v>
+        <v>48.015714286</v>
       </c>
     </row>
     <row r="90">
@@ -2225,19 +2225,19 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D90" t="n">
-        <v>0.004374832545153398</v>
+        <v>0.00240019628538921</v>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F90" t="n">
-        <v>45.56857143</v>
+        <v>48.61</v>
       </c>
     </row>
     <row r="91">
@@ -2245,19 +2245,19 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D91" t="n">
-        <v>0.002425314437850298</v>
+        <v>0.02004738767318043</v>
       </c>
       <c r="E91" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F91" t="n">
-        <v>83.52857143</v>
+        <v>48.61</v>
       </c>
     </row>
     <row r="92">
@@ -2265,19 +2265,19 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.002164504294690435</v>
+        <v>0.02484160924992753</v>
       </c>
       <c r="E92" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F92" t="n">
-        <v>87.95999999999999</v>
+        <v>47.818571429</v>
       </c>
     </row>
     <row r="93">
@@ -2285,19 +2285,19 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D93" t="n">
-        <v>0.001809954060799886</v>
+        <v>0.006341762531922348</v>
       </c>
       <c r="E93" t="n">
-        <v>2.5</v>
+        <v>34</v>
       </c>
       <c r="F93" t="n">
-        <v>87.95999999999999</v>
+        <v>49.54</v>
       </c>
     </row>
     <row r="94">
@@ -2305,19 +2305,19 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D94" t="n">
-        <v>0.002257188504255344</v>
+        <v>0.004039360578522472</v>
       </c>
       <c r="E94" t="n">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="F94" t="n">
-        <v>87.95999999999999</v>
+        <v>47.951428571</v>
       </c>
     </row>
     <row r="95">
@@ -2325,19 +2325,19 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.001884938557472164</v>
+        <v>0.003742992946637556</v>
       </c>
       <c r="E95" t="n">
-        <v>2.5</v>
+        <v>27</v>
       </c>
       <c r="F95" t="n">
-        <v>87.95999999999999</v>
+        <v>45.568571429</v>
       </c>
     </row>
     <row r="96">
@@ -2345,19 +2345,19 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0005584678690653593</v>
+        <v>0.008440493188665873</v>
       </c>
       <c r="E96" t="n">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="F96" t="n">
-        <v>87.95999999999999</v>
+        <v>49.54</v>
       </c>
     </row>
     <row r="97">
@@ -2365,19 +2365,19 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C97" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.0008196476953164111</v>
+        <v>0.01991904741416087</v>
       </c>
       <c r="E97" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F97" t="n">
-        <v>87.95999999999999</v>
+        <v>62.037142857</v>
       </c>
     </row>
     <row r="98">
@@ -2385,19 +2385,19 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D98" t="n">
-        <v>0.0001975073633468798</v>
+        <v>0.02572893309590481</v>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F98" t="n">
-        <v>87.95999999999999</v>
+        <v>78.7</v>
       </c>
     </row>
     <row r="99">
@@ -2405,19 +2405,19 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D99" t="n">
-        <v>0.008542583118458603</v>
+        <v>0.01992083323778775</v>
       </c>
       <c r="E99" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F99" t="n">
-        <v>76.84999999999999</v>
+        <v>78.7</v>
       </c>
     </row>
     <row r="100">
@@ -2425,19 +2425,19 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D100" t="n">
-        <v>0.003742419071212814</v>
+        <v>0.005286479339530283</v>
       </c>
       <c r="E100" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F100" t="n">
-        <v>76.84999999999999</v>
+        <v>78.7</v>
       </c>
     </row>
     <row r="101">
@@ -2445,19 +2445,19 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C101" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D101" t="n">
-        <v>-0.00179648881454896</v>
+        <v>0.005556197629816253</v>
       </c>
       <c r="E101" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F101" t="n">
-        <v>75.26428571</v>
+        <v>77.642857143</v>
       </c>
     </row>
     <row r="102">
@@ -2465,19 +2465,19 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C102" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D102" t="n">
-        <v>0.003715260180464124</v>
+        <v>0.01233426019797245</v>
       </c>
       <c r="E102" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F102" t="n">
-        <v>72.61714286</v>
+        <v>75</v>
       </c>
     </row>
     <row r="103">
@@ -2485,19 +2485,19 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D103" t="n">
-        <v>0.004346367490854344</v>
+        <v>0.008415870828738934</v>
       </c>
       <c r="E103" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="F103" t="n">
-        <v>72.22</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104">
@@ -2505,19 +2505,19 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D104" t="n">
-        <v>6.812733416237311e-05</v>
+        <v>0.009680382819717856</v>
       </c>
       <c r="E104" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F104" t="n">
-        <v>72.22</v>
+        <v>65.477142857</v>
       </c>
     </row>
     <row r="105">
@@ -2525,19 +2525,19 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D105" t="n">
-        <v>0.0002793221157102214</v>
+        <v>0.01147904732748661</v>
       </c>
       <c r="E105" t="n">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="F105" t="n">
-        <v>51.85</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="106">
@@ -2545,19 +2545,19 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D106" t="n">
-        <v>0.0004777066775761256</v>
+        <v>0.006436357158480325</v>
       </c>
       <c r="E106" t="n">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="F106" t="n">
-        <v>51.85</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="107">
@@ -2565,19 +2565,19 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D107" t="n">
-        <v>0.03778733060492338</v>
+        <v>0.005210144203667675</v>
       </c>
       <c r="E107" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F107" t="n">
-        <v>50.26428571</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="108">
@@ -2585,19 +2585,19 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D108" t="n">
-        <v>0.01173925917662048</v>
+        <v>0.03332145399187561</v>
       </c>
       <c r="E108" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F108" t="n">
-        <v>46.3</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="109">
@@ -2605,19 +2605,19 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D109" t="n">
-        <v>0.002663272823064753</v>
+        <v>0.01947487679103742</v>
       </c>
       <c r="E109" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F109" t="n">
-        <v>46.3</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="110">
@@ -2625,19 +2625,19 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D110" t="n">
-        <v>0.005109347817921268</v>
+        <v>0.004663629770938988</v>
       </c>
       <c r="E110" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F110" t="n">
-        <v>46.3</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="111">
@@ -2645,19 +2645,19 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D111" t="n">
-        <v>0.003632254264798749</v>
+        <v>0.0005189010792343414</v>
       </c>
       <c r="E111" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F111" t="n">
-        <v>46.3</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="112">
@@ -2665,19 +2665,19 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D112" t="n">
-        <v>0.00128150910474453</v>
+        <v>0.02013964665953423</v>
       </c>
       <c r="E112" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F112" t="n">
-        <v>47.09285714</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="113">
@@ -2685,19 +2685,19 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C113" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D113" t="n">
-        <v>0.04166407477706914</v>
+        <v>0.01461959034616894</v>
       </c>
       <c r="E113" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F113" t="n">
-        <v>48.15</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="114">
@@ -2705,19 +2705,19 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D114" t="n">
-        <v>0.04541542622075904</v>
+        <v>-0.001776756973831556</v>
       </c>
       <c r="E114" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F114" t="n">
-        <v>48.15</v>
+        <v>64.552857143</v>
       </c>
     </row>
     <row r="115">
@@ -2725,19 +2725,19 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D115" t="n">
-        <v>0.01511243422944563</v>
+        <v>0.002178137166467781</v>
       </c>
       <c r="E115" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F115" t="n">
-        <v>48.01571429</v>
+        <v>66.00714285700001</v>
       </c>
     </row>
     <row r="116">
@@ -2745,19 +2745,19 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C116" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D116" t="n">
-        <v>0.0014449953564092</v>
+        <v>-0.001029795664263842</v>
       </c>
       <c r="E116" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="F116" t="n">
-        <v>48.61</v>
+        <v>65.61</v>
       </c>
     </row>
     <row r="117">
@@ -2765,19 +2765,19 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C117" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D117" t="n">
-        <v>-0.0002356552773537571</v>
+        <v>-0.0007323480876772109</v>
       </c>
       <c r="E117" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F117" t="n">
-        <v>48.61</v>
+        <v>65.61</v>
       </c>
     </row>
     <row r="118">
@@ -2785,19 +2785,19 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D118" t="n">
-        <v>-0.0003708560320922171</v>
+        <v>0.006137471391615688</v>
       </c>
       <c r="E118" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F118" t="n">
-        <v>47.81857143</v>
+        <v>69.577142857</v>
       </c>
     </row>
     <row r="119">
@@ -2805,19 +2805,19 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D119" t="n">
-        <v>0.00181967023400513</v>
+        <v>0.005941977381314426</v>
       </c>
       <c r="E119" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F119" t="n">
-        <v>49.54</v>
+        <v>68.52</v>
       </c>
     </row>
     <row r="120">
@@ -2825,19 +2825,19 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D120" t="n">
-        <v>0.03167407367187682</v>
+        <v>-0.00163748306161212</v>
       </c>
       <c r="E120" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F120" t="n">
-        <v>47.95142857</v>
+        <v>74.471428571</v>
       </c>
     </row>
     <row r="121">
@@ -2845,19 +2845,19 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C121" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D121" t="n">
-        <v>0.02325131487667814</v>
+        <v>-0.002232984390673076</v>
       </c>
       <c r="E121" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F121" t="n">
-        <v>45.56857143</v>
+        <v>75</v>
       </c>
     </row>
     <row r="122">
@@ -2865,19 +2865,19 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C122" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D122" t="n">
-        <v>0.02369304310144036</v>
+        <v>0.00170187678530959</v>
       </c>
       <c r="E122" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F122" t="n">
-        <v>49.54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123">
@@ -2885,19 +2885,19 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C123" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D123" t="n">
-        <v>0.02763875377254164</v>
+        <v>0.002536824617437058</v>
       </c>
       <c r="E123" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F123" t="n">
-        <v>62.03714286</v>
+        <v>75</v>
       </c>
     </row>
     <row r="124">
@@ -2905,19 +2905,19 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C124" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D124" t="n">
-        <v>0.01774588829390188</v>
+        <v>0.004769043162502957</v>
       </c>
       <c r="E124" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F124" t="n">
-        <v>78.7</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="125">
@@ -2925,19 +2925,19 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C125" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D125" t="n">
-        <v>0.003445723832978797</v>
+        <v>0.00357582818916645</v>
       </c>
       <c r="E125" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F125" t="n">
-        <v>78.7</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="126">
@@ -2945,19 +2945,19 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D126" t="n">
-        <v>0.005274423260598064</v>
+        <v>0.003915403047328454</v>
       </c>
       <c r="E126" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F126" t="n">
-        <v>78.7</v>
+        <v>57.275714286</v>
       </c>
     </row>
     <row r="127">
@@ -2965,19 +2965,19 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C127" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D127" t="n">
-        <v>0.002435684459673785</v>
+        <v>0.03989961874293562</v>
       </c>
       <c r="E127" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F127" t="n">
-        <v>77.64285714</v>
+        <v>54.63</v>
       </c>
     </row>
     <row r="128">
@@ -2985,19 +2985,19 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C128" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D128" t="n">
-        <v>0.02299958822411221</v>
+        <v>0.02883803388008076</v>
       </c>
       <c r="E128" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F128" t="n">
-        <v>75</v>
+        <v>54.63</v>
       </c>
     </row>
     <row r="129">
@@ -3005,19 +3005,19 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D129" t="n">
-        <v>0.01884874974801482</v>
+        <v>0.003525533718181195</v>
       </c>
       <c r="E129" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F129" t="n">
-        <v>75</v>
+        <v>54.63</v>
       </c>
     </row>
     <row r="130">
@@ -3025,19 +3025,19 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C130" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D130" t="n">
-        <v>0.02057709826094441</v>
+        <v>0.005242502669970779</v>
       </c>
       <c r="E130" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F130" t="n">
-        <v>65.47714286</v>
+        <v>53.571428571</v>
       </c>
     </row>
     <row r="131">
@@ -3045,19 +3045,19 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="C131" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D131" t="n">
-        <v>0.01418674774741201</v>
+        <v>0.00252664614127105</v>
       </c>
       <c r="E131" t="n">
         <v>21</v>
       </c>
       <c r="F131" t="n">
-        <v>63.89</v>
+        <v>47.22</v>
       </c>
     </row>
     <row r="132">
@@ -3065,19 +3065,19 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1529411764705882</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D132" t="n">
-        <v>0.005331025503547773</v>
+        <v>0.0003633264883291852</v>
       </c>
       <c r="E132" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F132" t="n">
-        <v>63.89</v>
+        <v>46.227142857</v>
       </c>
     </row>
     <row r="133">
@@ -3085,19 +3085,19 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C133" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D133" t="n">
-        <v>0.002640671053001069</v>
+        <v>0.001638496014114538</v>
       </c>
       <c r="E133" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="F133" t="n">
-        <v>63.89</v>
+        <v>45.037142857</v>
       </c>
     </row>
     <row r="134">
@@ -3105,19 +3105,19 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C134" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D134" t="n">
-        <v>0.01660909501744489</v>
+        <v>-0.0009718491953527221</v>
       </c>
       <c r="E134" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F134" t="n">
-        <v>63.89</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="135">
@@ -3125,19 +3125,19 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C135" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D135" t="n">
-        <v>0.03638920783268147</v>
+        <v>-0.0001959984219566787</v>
       </c>
       <c r="E135" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F135" t="n">
-        <v>63.89</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="136">
@@ -3145,19 +3145,19 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D136" t="n">
-        <v>0.02468522351671784</v>
+        <v>0.004388529205399391</v>
       </c>
       <c r="E136" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="F136" t="n">
-        <v>63.89</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="137">
@@ -3165,19 +3165,19 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D137" t="n">
-        <v>0.0092389451671522</v>
+        <v>0.002806531671910708</v>
       </c>
       <c r="E137" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F137" t="n">
-        <v>63.89</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="138">
@@ -3185,19 +3185,19 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D138" t="n">
-        <v>0.001781193992222594</v>
+        <v>0.001195328656832604</v>
       </c>
       <c r="E138" t="n">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="F138" t="n">
-        <v>60.19</v>
+        <v>63.23</v>
       </c>
     </row>
     <row r="139">
@@ -3205,19 +3205,19 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D139" t="n">
-        <v>0.0423276384649877</v>
+        <v>0.003466010000233293</v>
       </c>
       <c r="E139" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F139" t="n">
-        <v>60.19</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="140">
@@ -3225,19 +3225,19 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D140" t="n">
-        <v>0.007778070734824855</v>
+        <v>0.00611872877958656</v>
       </c>
       <c r="E140" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F140" t="n">
-        <v>64.55285714</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="141">
@@ -3245,19 +3245,19 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D141" t="n">
-        <v>0.009290745794842011</v>
+        <v>0.009437216773441153</v>
       </c>
       <c r="E141" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F141" t="n">
-        <v>66.00714286</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="142">
@@ -3265,19 +3265,19 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D142" t="n">
-        <v>0.005218256361147928</v>
+        <v>0.02572519549787481</v>
       </c>
       <c r="E142" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="F142" t="n">
-        <v>65.61</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="143">
@@ -3285,19 +3285,19 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C143" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D143" t="n">
-        <v>-0.0003221390198496134</v>
+        <v>0.01983001611181059</v>
       </c>
       <c r="E143" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F143" t="n">
-        <v>65.61</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="144">
@@ -3305,19 +3305,19 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D144" t="n">
-        <v>0.01195545573602142</v>
+        <v>0.02204899960548908</v>
       </c>
       <c r="E144" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F144" t="n">
-        <v>69.57714286</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="145">
@@ -3325,19 +3325,19 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C145" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D145" t="n">
-        <v>0.0076394863040195</v>
+        <v>0.006443136781049377</v>
       </c>
       <c r="E145" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F145" t="n">
-        <v>68.52</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="146">
@@ -3345,19 +3345,19 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D146" t="n">
-        <v>0.03120819497867222</v>
+        <v>0.004208670827036078</v>
       </c>
       <c r="E146" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="F146" t="n">
-        <v>74.47142857</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="147">
@@ -3365,19 +3365,19 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C147" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D147" t="n">
-        <v>0.02026337723711574</v>
+        <v>0.007234712693020596</v>
       </c>
       <c r="E147" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F147" t="n">
-        <v>75</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="148">
@@ -3385,19 +3385,19 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C148" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D148" t="n">
-        <v>0.01679878575462652</v>
+        <v>0.00637820154581309</v>
       </c>
       <c r="E148" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F148" t="n">
-        <v>75</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="149">
@@ -3405,19 +3405,19 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1294117647058824</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D149" t="n">
-        <v>0.01704917158010017</v>
+        <v>0.008585421285848559</v>
       </c>
       <c r="E149" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F149" t="n">
-        <v>75</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="150">
@@ -3425,19 +3425,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C150" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D150" t="n">
-        <v>0.008906901393395212</v>
+        <v>0.01438861513226988</v>
       </c>
       <c r="E150" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F150" t="n">
-        <v>63.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="151">
@@ -3445,19 +3445,19 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D151" t="n">
-        <v>0.01912165225246047</v>
+        <v>0.0226615546711354</v>
       </c>
       <c r="E151" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="F151" t="n">
-        <v>63.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="152">
@@ -3465,19 +3465,19 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C152" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D152" t="n">
-        <v>0.01604441312553097</v>
+        <v>0.01801665905055521</v>
       </c>
       <c r="E152" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F152" t="n">
-        <v>57.27571429</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="153">
@@ -3485,19 +3485,19 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C153" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D153" t="n">
-        <v>0.002351340470293178</v>
+        <v>0.007741085183371643</v>
       </c>
       <c r="E153" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F153" t="n">
-        <v>54.63</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="154">
@@ -3505,19 +3505,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C154" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D154" t="n">
-        <v>-0.0009081685558169261</v>
+        <v>0.05531676109754369</v>
       </c>
       <c r="E154" t="n">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="F154" t="n">
-        <v>54.63</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="155">
@@ -3525,19 +3525,19 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C155" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D155" t="n">
-        <v>0.007826482013880004</v>
+        <v>0.03055054310141514</v>
       </c>
       <c r="E155" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="F155" t="n">
-        <v>54.63</v>
+        <v>65.9725</v>
       </c>
     </row>
     <row r="156">
@@ -3545,19 +3545,19 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C156" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D156" t="n">
-        <v>0.004874865433115444</v>
+        <v>0.04636428342294657</v>
       </c>
       <c r="E156" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="F156" t="n">
-        <v>53.57142857</v>
+        <v>72.22</v>
       </c>
     </row>
     <row r="157">
@@ -3565,19 +3565,19 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C157" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D157" t="n">
-        <v>0.002061891800982244</v>
+        <v>0.0489392845843442</v>
       </c>
       <c r="E157" t="n">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="F157" t="n">
-        <v>47.22</v>
+        <v>72.22</v>
       </c>
     </row>
     <row r="158">
@@ -3585,19 +3585,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C158" t="n">
-        <v>0.1411764705882353</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="D158" t="n">
-        <v>-0.0005154729502455903</v>
+        <v>0.04535333011523631</v>
       </c>
       <c r="E158" t="n">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="F158" t="n">
-        <v>46.22714286</v>
+        <v>72.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>